<commit_message>
fixes and other things
</commit_message>
<xml_diff>
--- a/REST_files/WorkCenters.xlsx
+++ b/REST_files/WorkCenters.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1745,7 +1745,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>BIG BAG LINE BAXTER SPRINGS</t>
+          <t>BAXTER BIG BAG - LINE 2</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>PARSONS BAXTER SPRINGS</t>
+          <t>BAXTER SMALL BAG -  LINE 1</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1969,6 +1969,50 @@
         </is>
       </c>
       <c r="D70" t="inlineStr">
+        <is>
+          <t>PACK</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>20005</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>74510</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>SUP PAWNEE CITY</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>PACK</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>20005</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>74511</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>PSGLEE PAWNEE CITY</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
         <is>
           <t>PACK</t>
         </is>

</xml_diff>